<commit_message>
update gender column to use F or M
</commit_message>
<xml_diff>
--- a/src/main/resources/data/events.xlsx
+++ b/src/main/resources/data/events.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YOUNEVSKY\Desktop\S4\stage\excel-to-db\excel-to-db\src\main\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YOUNEVSKY\Desktop\S4\stage\excel-to-db\excel-to-db\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B72BED1-F7B5-4059-B8C5-E2FC3E04D3A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7580FA10-FE66-4052-BE45-90B3050011C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{BC3EBE38-1540-4038-95AB-EDE7D7A42B8D}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>elhasnaoui</t>
   </si>
   <si>
-    <t>male</t>
-  </si>
-  <si>
     <t>casablanca</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>s.issaoui@gmail.com</t>
   </si>
   <si>
-    <t>female</t>
-  </si>
-  <si>
     <t>fes</t>
   </si>
   <si>
@@ -166,6 +160,12 @@
   </si>
   <si>
     <t>event_users_count</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -173,7 +173,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ am/pm"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -216,8 +216,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -556,7 +556,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,37 +573,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>32</v>
-      </c>
-      <c r="J1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -617,7 +617,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2">
         <v>2004</v>
@@ -629,16 +629,16 @@
         <v>9</v>
       </c>
       <c r="H2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" t="s">
         <v>2</v>
-      </c>
-      <c r="I2" t="s">
-        <v>3</v>
       </c>
       <c r="J2">
         <v>100</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -646,13 +646,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3">
         <v>2003</v>
@@ -664,16 +664,16 @@
         <v>29</v>
       </c>
       <c r="H3" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J3">
         <v>100</v>
       </c>
       <c r="K3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -681,13 +681,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <v>1999</v>
@@ -699,16 +699,16 @@
         <v>12</v>
       </c>
       <c r="H4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" t="s">
         <v>19</v>
-      </c>
-      <c r="I4" t="s">
-        <v>21</v>
       </c>
       <c r="J4">
         <v>100</v>
       </c>
       <c r="K4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -716,13 +716,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5">
         <v>1997</v>
@@ -734,16 +734,16 @@
         <v>10</v>
       </c>
       <c r="H5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" t="s">
         <v>2</v>
-      </c>
-      <c r="I5" t="s">
-        <v>3</v>
       </c>
       <c r="J5">
         <v>100</v>
       </c>
       <c r="K5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -751,13 +751,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6">
         <v>2000</v>
@@ -769,16 +769,16 @@
         <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="I6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J6">
         <v>100</v>
       </c>
       <c r="K6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -809,34 +809,34 @@
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>36</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>38</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>39</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>40</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -844,21 +844,21 @@
         <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>2024</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>4</v>
       </c>
       <c r="F2">
         <v>25</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>0.4375</v>
       </c>
       <c r="H2">

</xml_diff>

<commit_message>
remove old structure (classes)
</commit_message>
<xml_diff>
--- a/src/main/resources/data/events.xlsx
+++ b/src/main/resources/data/events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YOUNEVSKY\Desktop\S4\stage\excel-to-db\excel-to-db\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7580FA10-FE66-4052-BE45-90B3050011C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513AC46E-3486-4188-8A15-BBE5286A7CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{BC3EBE38-1540-4038-95AB-EDE7D7A42B8D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{BC3EBE38-1540-4038-95AB-EDE7D7A42B8D}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -555,7 +555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C6386D-85D0-4167-AD7D-B463160FDF75}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -798,7 +798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDEF9BAD-3EE3-41D2-8ADA-49E73FC97A1C}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>

</xml_diff>